<commit_message>
bug on network of model is fixed. but there is another bug on NMS.
</commit_message>
<xml_diff>
--- a/tools/yolov3-spp.xlsx
+++ b/tools/yolov3-spp.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maruyama/Projects/private/public/yolo_various_platforms/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{657F9F35-39A6-BA49-B2BF-74A113999816}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D352569-E465-364A-8F0D-11A0982FCF2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="20" windowWidth="28300" windowHeight="17440"/>
+    <workbookView xWindow="500" yWindow="20" windowWidth="28300" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yolov3-spp" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -328,7 +328,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +514,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -631,40 +661,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="8"/>
+      <left style="thin">
+        <color theme="3"/>
       </left>
-      <right style="medium">
-        <color theme="8"/>
+      <right style="thin">
+        <color theme="3"/>
       </right>
-      <top style="medium">
-        <color theme="8"/>
+      <top style="thin">
+        <color theme="3"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="8"/>
+      <left style="thin">
+        <color theme="3"/>
       </left>
-      <right style="medium">
-        <color theme="8"/>
-      </right>
-      <top/>
-      <bottom/>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="8"/>
+      <left style="thin">
+        <color theme="3"/>
       </left>
-      <right style="medium">
-        <color theme="8"/>
+      <right style="thin">
+        <color theme="3"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -796,24 +830,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1169,11 +1236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="L93" sqref="L93:N94"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1216,11 +1283,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
       <c r="O1" t="s">
         <v>32</v>
       </c>
@@ -1253,15 +1320,15 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21" thickBot="1">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1359,7 @@
       <c r="L3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N3" s="4"/>
@@ -1328,7 +1395,7 @@
       <c r="L4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="4"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:15">
@@ -1360,10 +1427,10 @@
         <v>3</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="12"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="21" thickBot="1">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1376,11 +1443,11 @@
       <c r="J6">
         <v>-3</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="4"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="21" thickBot="1">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1411,7 +1478,7 @@
       <c r="L7" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N7" s="4"/>
@@ -1447,7 +1514,7 @@
       <c r="L8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="12"/>
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:15">
@@ -1479,10 +1546,10 @@
         <v>7</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="12"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="21" thickBot="1">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1495,8 +1562,8 @@
       <c r="J10">
         <v>-3</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="12"/>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:15">
@@ -1530,7 +1597,7 @@
       <c r="L11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="12"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:15">
@@ -1562,10 +1629,10 @@
         <v>10</v>
       </c>
       <c r="L12" s="2"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="12"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:15" ht="21" thickBot="1">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1578,11 +1645,11 @@
       <c r="J13">
         <v>-3</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="4"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="12"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="21" thickBot="1">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1680,7 @@
       <c r="L14" t="s">
         <v>30</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N14" s="4"/>
@@ -1649,7 +1716,7 @@
       <c r="L15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="12"/>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:15">
@@ -1681,10 +1748,10 @@
         <v>14</v>
       </c>
       <c r="L16" s="2"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="12"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" ht="21" thickBot="1">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1697,8 +1764,8 @@
       <c r="J17">
         <v>-3</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="4"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="12"/>
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14">
@@ -1732,7 +1799,7 @@
       <c r="L18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="12"/>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14">
@@ -1764,10 +1831,10 @@
         <v>17</v>
       </c>
       <c r="L19" s="2"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" ht="21" thickBot="1">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1780,8 +1847,8 @@
       <c r="J20">
         <v>-3</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="4"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="12"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14">
@@ -1815,7 +1882,7 @@
       <c r="L21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="12"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14">
@@ -1847,10 +1914,10 @@
         <v>20</v>
       </c>
       <c r="L22" s="2"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="12"/>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="1:14" ht="21" thickBot="1">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1863,8 +1930,8 @@
       <c r="J23">
         <v>-3</v>
       </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="4"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="12"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14">
@@ -1898,7 +1965,7 @@
       <c r="L24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="4"/>
+      <c r="M24" s="12"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14">
@@ -1930,10 +1997,10 @@
         <v>23</v>
       </c>
       <c r="L25" s="2"/>
-      <c r="M25" s="4"/>
+      <c r="M25" s="12"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" ht="21" thickBot="1">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1946,8 +2013,8 @@
       <c r="J26">
         <v>-3</v>
       </c>
-      <c r="L26" s="3"/>
-      <c r="M26" s="4"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="12"/>
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="1:14">
@@ -1981,7 +2048,7 @@
       <c r="L27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="4"/>
+      <c r="M27" s="12"/>
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:14">
@@ -2013,10 +2080,10 @@
         <v>26</v>
       </c>
       <c r="L28" s="2"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="12"/>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:14" ht="21" thickBot="1">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2029,8 +2096,8 @@
       <c r="J29">
         <v>-3</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="4"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="12"/>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14">
@@ -2064,7 +2131,7 @@
       <c r="L30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M30" s="4"/>
+      <c r="M30" s="12"/>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:14">
@@ -2096,10 +2163,10 @@
         <v>29</v>
       </c>
       <c r="L31" s="2"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="12"/>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:14" ht="21" thickBot="1">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2112,8 +2179,8 @@
       <c r="J32">
         <v>-3</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="4"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="12"/>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14">
@@ -2147,7 +2214,7 @@
       <c r="L33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M33" s="4"/>
+      <c r="M33" s="12"/>
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14">
@@ -2179,10 +2246,10 @@
         <v>32</v>
       </c>
       <c r="L34" s="2"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="12"/>
       <c r="N34" s="4"/>
     </row>
-    <row r="35" spans="1:14" ht="21" thickBot="1">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2195,8 +2262,8 @@
       <c r="J35">
         <v>-3</v>
       </c>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="12"/>
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:14">
@@ -2230,7 +2297,7 @@
       <c r="L36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="4"/>
+      <c r="M36" s="12"/>
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:14">
@@ -2262,27 +2329,27 @@
         <v>35</v>
       </c>
       <c r="L37" s="2"/>
-      <c r="M37" s="4"/>
+      <c r="M37" s="12"/>
       <c r="N37" s="4"/>
     </row>
-    <row r="38" spans="1:14" ht="21" thickBot="1">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="G38" t="s">
         <v>14</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="16">
         <v>36</v>
       </c>
       <c r="J38">
         <v>-3</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="4"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="12"/>
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="1:14" ht="21" thickBot="1">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2313,7 +2380,7 @@
       <c r="L39" t="s">
         <v>30</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M39" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N39" s="4"/>
@@ -2349,7 +2416,7 @@
       <c r="L40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M40" s="4"/>
+      <c r="M40" s="13"/>
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:14">
@@ -2381,10 +2448,10 @@
         <v>39</v>
       </c>
       <c r="L41" s="2"/>
-      <c r="M41" s="4"/>
+      <c r="M41" s="13"/>
       <c r="N41" s="4"/>
     </row>
-    <row r="42" spans="1:14" ht="21" thickBot="1">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2397,8 +2464,8 @@
       <c r="J42">
         <v>-3</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="4"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="13"/>
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="1:14">
@@ -2432,7 +2499,7 @@
       <c r="L43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M43" s="4"/>
+      <c r="M43" s="13"/>
       <c r="N43" s="4"/>
     </row>
     <row r="44" spans="1:14">
@@ -2464,10 +2531,10 @@
         <v>42</v>
       </c>
       <c r="L44" s="2"/>
-      <c r="M44" s="4"/>
+      <c r="M44" s="13"/>
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="1:14" ht="21" thickBot="1">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -2480,8 +2547,8 @@
       <c r="J45">
         <v>-3</v>
       </c>
-      <c r="L45" s="3"/>
-      <c r="M45" s="4"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="13"/>
       <c r="N45" s="4"/>
     </row>
     <row r="46" spans="1:14">
@@ -2515,7 +2582,7 @@
       <c r="L46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M46" s="4"/>
+      <c r="M46" s="13"/>
       <c r="N46" s="4"/>
     </row>
     <row r="47" spans="1:14">
@@ -2547,10 +2614,10 @@
         <v>45</v>
       </c>
       <c r="L47" s="2"/>
-      <c r="M47" s="4"/>
+      <c r="M47" s="13"/>
       <c r="N47" s="4"/>
     </row>
-    <row r="48" spans="1:14" ht="21" thickBot="1">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2563,8 +2630,8 @@
       <c r="J48">
         <v>-3</v>
       </c>
-      <c r="L48" s="3"/>
-      <c r="M48" s="4"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="13"/>
       <c r="N48" s="4"/>
     </row>
     <row r="49" spans="1:14">
@@ -2598,7 +2665,7 @@
       <c r="L49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M49" s="4"/>
+      <c r="M49" s="13"/>
       <c r="N49" s="4"/>
     </row>
     <row r="50" spans="1:14">
@@ -2630,10 +2697,10 @@
         <v>48</v>
       </c>
       <c r="L50" s="2"/>
-      <c r="M50" s="4"/>
+      <c r="M50" s="13"/>
       <c r="N50" s="4"/>
     </row>
-    <row r="51" spans="1:14" ht="21" thickBot="1">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -2646,8 +2713,8 @@
       <c r="J51">
         <v>-3</v>
       </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="4"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="13"/>
       <c r="N51" s="4"/>
     </row>
     <row r="52" spans="1:14">
@@ -2681,7 +2748,7 @@
       <c r="L52" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M52" s="4"/>
+      <c r="M52" s="13"/>
       <c r="N52" s="4"/>
     </row>
     <row r="53" spans="1:14">
@@ -2713,10 +2780,10 @@
         <v>51</v>
       </c>
       <c r="L53" s="2"/>
-      <c r="M53" s="4"/>
+      <c r="M53" s="13"/>
       <c r="N53" s="4"/>
     </row>
-    <row r="54" spans="1:14" ht="21" thickBot="1">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -2729,8 +2796,8 @@
       <c r="J54">
         <v>-3</v>
       </c>
-      <c r="L54" s="3"/>
-      <c r="M54" s="4"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="13"/>
       <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:14">
@@ -2764,7 +2831,7 @@
       <c r="L55" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M55" s="4"/>
+      <c r="M55" s="13"/>
       <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:14">
@@ -2796,10 +2863,10 @@
         <v>54</v>
       </c>
       <c r="L56" s="2"/>
-      <c r="M56" s="4"/>
+      <c r="M56" s="13"/>
       <c r="N56" s="4"/>
     </row>
-    <row r="57" spans="1:14" ht="21" thickBot="1">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -2812,8 +2879,8 @@
       <c r="J57">
         <v>-3</v>
       </c>
-      <c r="L57" s="3"/>
-      <c r="M57" s="4"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="13"/>
       <c r="N57" s="4"/>
     </row>
     <row r="58" spans="1:14">
@@ -2847,7 +2914,7 @@
       <c r="L58" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M58" s="4"/>
+      <c r="M58" s="13"/>
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:14">
@@ -2879,10 +2946,10 @@
         <v>57</v>
       </c>
       <c r="L59" s="2"/>
-      <c r="M59" s="4"/>
+      <c r="M59" s="13"/>
       <c r="N59" s="4"/>
     </row>
-    <row r="60" spans="1:14" ht="21" thickBot="1">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -2895,8 +2962,8 @@
       <c r="J60">
         <v>-3</v>
       </c>
-      <c r="L60" s="3"/>
-      <c r="M60" s="4"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="13"/>
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:14">
@@ -2930,7 +2997,7 @@
       <c r="L61" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M61" s="4"/>
+      <c r="M61" s="13"/>
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="1:14">
@@ -2962,27 +3029,27 @@
         <v>60</v>
       </c>
       <c r="L62" s="2"/>
-      <c r="M62" s="4"/>
+      <c r="M62" s="13"/>
       <c r="N62" s="4"/>
     </row>
-    <row r="63" spans="1:14" ht="21" thickBot="1">
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>13</v>
       </c>
       <c r="G63" t="s">
         <v>14</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="16">
         <v>61</v>
       </c>
       <c r="J63">
         <v>-3</v>
       </c>
-      <c r="L63" s="3"/>
-      <c r="M63" s="4"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="13"/>
       <c r="N63" s="4"/>
     </row>
-    <row r="64" spans="1:14" ht="21" thickBot="1">
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -3013,7 +3080,7 @@
       <c r="L64" t="s">
         <v>30</v>
       </c>
-      <c r="M64" s="5" t="s">
+      <c r="M64" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N64" s="4"/>
@@ -3046,10 +3113,10 @@
       <c r="I65">
         <v>63</v>
       </c>
-      <c r="L65" s="1" t="s">
+      <c r="L65" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M65" s="4"/>
+      <c r="M65" s="14"/>
       <c r="N65" s="4"/>
     </row>
     <row r="66" spans="1:14">
@@ -3080,11 +3147,11 @@
       <c r="I66">
         <v>64</v>
       </c>
-      <c r="L66" s="2"/>
-      <c r="M66" s="4"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="14"/>
       <c r="N66" s="4"/>
     </row>
-    <row r="67" spans="1:14" ht="21" thickBot="1">
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -3097,8 +3164,8 @@
       <c r="J67">
         <v>-3</v>
       </c>
-      <c r="L67" s="3"/>
-      <c r="M67" s="4"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="14"/>
       <c r="N67" s="4"/>
     </row>
     <row r="68" spans="1:14">
@@ -3129,10 +3196,10 @@
       <c r="I68">
         <v>66</v>
       </c>
-      <c r="L68" s="1" t="s">
+      <c r="L68" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M68" s="4"/>
+      <c r="M68" s="14"/>
       <c r="N68" s="4"/>
     </row>
     <row r="69" spans="1:14">
@@ -3163,11 +3230,11 @@
       <c r="I69">
         <v>67</v>
       </c>
-      <c r="L69" s="2"/>
-      <c r="M69" s="4"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="14"/>
       <c r="N69" s="4"/>
     </row>
-    <row r="70" spans="1:14" ht="21" thickBot="1">
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -3180,8 +3247,8 @@
       <c r="J70">
         <v>-3</v>
       </c>
-      <c r="L70" s="3"/>
-      <c r="M70" s="4"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="14"/>
       <c r="N70" s="4"/>
     </row>
     <row r="71" spans="1:14">
@@ -3212,10 +3279,10 @@
       <c r="I71">
         <v>69</v>
       </c>
-      <c r="L71" s="1" t="s">
+      <c r="L71" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M71" s="4"/>
+      <c r="M71" s="14"/>
       <c r="N71" s="4"/>
     </row>
     <row r="72" spans="1:14">
@@ -3246,11 +3313,11 @@
       <c r="I72">
         <v>70</v>
       </c>
-      <c r="L72" s="2"/>
-      <c r="M72" s="4"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="14"/>
       <c r="N72" s="4"/>
     </row>
-    <row r="73" spans="1:14" ht="21" thickBot="1">
+    <row r="73" spans="1:14">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -3263,8 +3330,8 @@
       <c r="J73">
         <v>-3</v>
       </c>
-      <c r="L73" s="3"/>
-      <c r="M73" s="4"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="14"/>
       <c r="N73" s="4"/>
     </row>
     <row r="74" spans="1:14">
@@ -3295,10 +3362,10 @@
       <c r="I74">
         <v>72</v>
       </c>
-      <c r="L74" s="1" t="s">
+      <c r="L74" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M74" s="4"/>
+      <c r="M74" s="14"/>
       <c r="N74" s="4"/>
     </row>
     <row r="75" spans="1:14">
@@ -3329,11 +3396,11 @@
       <c r="I75">
         <v>73</v>
       </c>
-      <c r="L75" s="2"/>
-      <c r="M75" s="4"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="14"/>
       <c r="N75" s="4"/>
     </row>
-    <row r="76" spans="1:14" ht="21" thickBot="1">
+    <row r="76" spans="1:14">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -3346,8 +3413,8 @@
       <c r="J76">
         <v>-3</v>
       </c>
-      <c r="L76" s="3"/>
-      <c r="M76" s="4"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="14"/>
       <c r="N76" s="4"/>
     </row>
     <row r="77" spans="1:14">
@@ -3378,10 +3445,10 @@
       <c r="I77">
         <v>75</v>
       </c>
-      <c r="L77" s="4" t="s">
+      <c r="L77" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M77" s="4"/>
+      <c r="M77" s="5"/>
       <c r="N77" s="4"/>
     </row>
     <row r="78" spans="1:14">
@@ -3412,8 +3479,8 @@
       <c r="I78">
         <v>76</v>
       </c>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
       <c r="N78" s="4"/>
     </row>
     <row r="79" spans="1:14">
@@ -3444,8 +3511,8 @@
       <c r="I79">
         <v>77</v>
       </c>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
       <c r="N79" s="4"/>
     </row>
     <row r="80" spans="1:14">
@@ -3461,8 +3528,8 @@
       <c r="I80">
         <v>78</v>
       </c>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
       <c r="N80" s="4"/>
     </row>
     <row r="81" spans="1:15">
@@ -3475,8 +3542,8 @@
       <c r="K81">
         <v>-2</v>
       </c>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
       <c r="N81" s="4"/>
     </row>
     <row r="82" spans="1:15">
@@ -3492,8 +3559,8 @@
       <c r="I82">
         <v>80</v>
       </c>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
       <c r="N82" s="4"/>
     </row>
     <row r="83" spans="1:15">
@@ -3506,8 +3573,8 @@
       <c r="K83">
         <v>-4</v>
       </c>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
       <c r="N83" s="4"/>
     </row>
     <row r="84" spans="1:15">
@@ -3523,8 +3590,8 @@
       <c r="I84">
         <v>82</v>
       </c>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
       <c r="N84" s="4"/>
     </row>
     <row r="85" spans="1:15">
@@ -3537,8 +3604,8 @@
       <c r="K85" t="s">
         <v>17</v>
       </c>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
       <c r="N85" s="4"/>
     </row>
     <row r="86" spans="1:15">
@@ -3569,8 +3636,8 @@
       <c r="I86">
         <v>84</v>
       </c>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
+      <c r="L86" s="5"/>
+      <c r="M86" s="5"/>
       <c r="N86" s="4"/>
     </row>
     <row r="87" spans="1:15">
@@ -3601,8 +3668,8 @@
       <c r="I87">
         <v>85</v>
       </c>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
       <c r="N87" s="4"/>
     </row>
     <row r="88" spans="1:15">
@@ -3630,11 +3697,11 @@
       <c r="H88">
         <v>1</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="16">
         <v>86</v>
       </c>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
       <c r="N88" s="4"/>
     </row>
     <row r="89" spans="1:15">
@@ -3756,11 +3823,11 @@
       <c r="I93">
         <v>91</v>
       </c>
-      <c r="L93" s="4" t="s">
+      <c r="L93" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M93" s="4"/>
-      <c r="N93" s="4"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
     </row>
     <row r="94" spans="1:15">
       <c r="A94" t="s">
@@ -3772,9 +3839,9 @@
       <c r="I94">
         <v>92</v>
       </c>
-      <c r="L94" s="4"/>
-      <c r="M94" s="4"/>
-      <c r="N94" s="4"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
     </row>
     <row r="95" spans="1:15">
       <c r="A95" t="s">
@@ -3818,11 +3885,11 @@
       <c r="I96">
         <v>94</v>
       </c>
-      <c r="L96" s="4" t="s">
+      <c r="L96" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M96" s="4"/>
-      <c r="N96" s="4"/>
+      <c r="M96" s="7"/>
+      <c r="N96" s="7"/>
     </row>
     <row r="97" spans="1:15">
       <c r="A97" t="s">
@@ -3852,9 +3919,9 @@
       <c r="I97">
         <v>95</v>
       </c>
-      <c r="L97" s="4"/>
-      <c r="M97" s="4"/>
-      <c r="N97" s="4"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="7"/>
+      <c r="N97" s="7"/>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" t="s">
@@ -3884,9 +3951,9 @@
       <c r="I98">
         <v>96</v>
       </c>
-      <c r="L98" s="4"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="4"/>
+      <c r="L98" s="7"/>
+      <c r="M98" s="7"/>
+      <c r="N98" s="7"/>
     </row>
     <row r="99" spans="1:15">
       <c r="A99" t="s">
@@ -3916,9 +3983,9 @@
       <c r="I99">
         <v>97</v>
       </c>
-      <c r="L99" s="4"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="7"/>
+      <c r="N99" s="7"/>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" t="s">
@@ -3945,12 +4012,12 @@
       <c r="H100">
         <v>1</v>
       </c>
-      <c r="I100">
+      <c r="I100" s="16">
         <v>98</v>
       </c>
-      <c r="L100" s="4"/>
-      <c r="M100" s="4"/>
-      <c r="N100" s="4"/>
+      <c r="L100" s="7"/>
+      <c r="M100" s="7"/>
+      <c r="N100" s="7"/>
     </row>
     <row r="101" spans="1:15">
       <c r="A101" t="s">
@@ -4071,11 +4138,11 @@
       <c r="I105">
         <v>103</v>
       </c>
-      <c r="L105" s="4" t="s">
+      <c r="L105" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
     </row>
     <row r="106" spans="1:15">
       <c r="A106" t="s">
@@ -4087,9 +4154,9 @@
       <c r="I106">
         <v>104</v>
       </c>
-      <c r="L106" s="4"/>
-      <c r="M106" s="4"/>
-      <c r="N106" s="4"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
     </row>
     <row r="107" spans="1:15">
       <c r="A107" t="s">
@@ -4133,11 +4200,11 @@
       <c r="I108">
         <v>106</v>
       </c>
-      <c r="L108" s="4" t="s">
+      <c r="L108" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M108" s="4"/>
-      <c r="N108" s="4"/>
+      <c r="M108" s="7"/>
+      <c r="N108" s="7"/>
     </row>
     <row r="109" spans="1:15">
       <c r="A109" t="s">
@@ -4167,9 +4234,9 @@
       <c r="I109">
         <v>107</v>
       </c>
-      <c r="L109" s="4"/>
-      <c r="M109" s="4"/>
-      <c r="N109" s="4"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="7"/>
+      <c r="N109" s="7"/>
     </row>
     <row r="110" spans="1:15">
       <c r="A110" t="s">
@@ -4199,9 +4266,9 @@
       <c r="I110">
         <v>108</v>
       </c>
-      <c r="L110" s="4"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="4"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="7"/>
+      <c r="N110" s="7"/>
     </row>
     <row r="111" spans="1:15">
       <c r="A111" t="s">
@@ -4231,9 +4298,9 @@
       <c r="I111">
         <v>109</v>
       </c>
-      <c r="L111" s="4"/>
-      <c r="M111" s="4"/>
-      <c r="N111" s="4"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="7"/>
+      <c r="N111" s="7"/>
     </row>
     <row r="112" spans="1:15">
       <c r="A112" t="s">
@@ -4263,9 +4330,9 @@
       <c r="I112">
         <v>110</v>
       </c>
-      <c r="L112" s="4"/>
-      <c r="M112" s="4"/>
-      <c r="N112" s="4"/>
+      <c r="L112" s="7"/>
+      <c r="M112" s="7"/>
+      <c r="N112" s="7"/>
     </row>
     <row r="113" spans="1:15">
       <c r="A113" t="s">
@@ -4351,12 +4418,22 @@
     <mergeCell ref="L113:N115"/>
     <mergeCell ref="N2:N88"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L101:N103"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="L49:L51"/>
+    <mergeCell ref="L52:L54"/>
+    <mergeCell ref="L55:L57"/>
+    <mergeCell ref="L58:L60"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="L27:L29"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="L33:L35"/>
+    <mergeCell ref="L36:L38"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="L89:N91"/>
     <mergeCell ref="L77:M88"/>
     <mergeCell ref="L93:N94"/>
     <mergeCell ref="L96:N100"/>
-    <mergeCell ref="L101:N103"/>
     <mergeCell ref="L61:L63"/>
     <mergeCell ref="L65:L67"/>
     <mergeCell ref="L68:L70"/>
@@ -4368,16 +4445,6 @@
     <mergeCell ref="M39:M63"/>
     <mergeCell ref="M64:M76"/>
     <mergeCell ref="L43:L45"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="L49:L51"/>
-    <mergeCell ref="L52:L54"/>
-    <mergeCell ref="L55:L57"/>
-    <mergeCell ref="L58:L60"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="L27:L29"/>
-    <mergeCell ref="L30:L32"/>
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="L36:L38"/>
     <mergeCell ref="L40:L42"/>
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="L8:L10"/>

</xml_diff>